<commit_message>
Bug fix #44 enhancement #46
- close #44: fix url path in ajax petitions para plantilla PL2
- close #46: página agradecimiento añadida a PL0
</commit_message>
<xml_diff>
--- a/docs/Variables_(CodeOP).xlsx
+++ b/docs/Variables_(CodeOP).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="246">
   <si>
     <t>TmpTotal</t>
   </si>
@@ -747,6 +747,12 @@
   </si>
   <si>
     <t>Registra el momento en que se termina de leer el FDBK</t>
+  </si>
+  <si>
+    <t>Fin de realización de Grupo (después de la página de agradecimiento)</t>
+  </si>
+  <si>
+    <t>FinGrupoAgrad</t>
   </si>
 </sst>
 </file>
@@ -2793,7 +2799,7 @@
   <dimension ref="A1:K73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,7 +2807,8 @@
     <col min="1" max="1" width="11.42578125" style="30"/>
     <col min="2" max="3" width="18.140625" style="30" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="47.42578125" customWidth="1"/>
+    <col min="6" max="8" width="26.7109375" customWidth="1"/>
     <col min="9" max="9" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="82.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.140625" style="31" bestFit="1" customWidth="1"/>
@@ -4753,7 +4760,7 @@
     </row>
     <row r="65" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="50">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B65" s="50" t="s">
         <v>241</v>
@@ -4773,15 +4780,24 @@
       <c r="K65" s="53"/>
     </row>
     <row r="66" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="50"/>
-      <c r="B66" s="50"/>
-      <c r="C66" s="50"/>
+      <c r="A66" s="50">
+        <v>130</v>
+      </c>
+      <c r="B66" s="50" t="s">
+        <v>245</v>
+      </c>
+      <c r="C66" s="50" t="s">
+        <v>159</v>
+      </c>
       <c r="D66" s="52"/>
       <c r="E66" s="52"/>
       <c r="F66" s="52"/>
       <c r="G66" s="52"/>
       <c r="H66" s="52"/>
       <c r="I66" s="52"/>
+      <c r="J66" s="49" t="s">
+        <v>244</v>
+      </c>
       <c r="K66" s="53"/>
     </row>
     <row r="67" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>